<commit_message>
EXPERIMENTAL - Finalized ISR with Quote Widget and added Fetched On Context
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Work\Programming\Projects\briefme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Work\Programming\Projects\brief-me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015D8D06-1B3C-4A74-85D2-F793DDC712FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44EB9F6-8BC2-4EB2-B6E7-BC77B87F3B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="135">
   <si>
     <t>Feature</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/api/rest_v1/feed/onthisday/holidays/01/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Current Time/Day</t>
+  </si>
+  <si>
+    <t>https://worldtimeapi.org/api/timezone/Asia/Kolkata</t>
   </si>
 </sst>
 </file>
@@ -839,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,143 +1297,164 @@
       <c r="E13" s="3"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="5" t="s">
+      <c r="E15" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N15" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.850000000000001" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:14" ht="17.850000000000001" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="5">
-        <v>7</v>
-      </c>
-      <c r="N17" s="5">
-        <v>4</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="M18" s="5">
+        <v>7</v>
+      </c>
+      <c r="N18" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M24" s="5"/>
-    </row>
-    <row r="27" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1436,20 +1466,21 @@
     <hyperlink ref="D3" r:id="rId4" xr:uid="{15D4EC06-BDF0-49DB-81D8-16C0A8C105FF}"/>
     <hyperlink ref="L3" r:id="rId5" xr:uid="{BD1FCE84-4B18-4DAE-BECD-AE06A5B4B331}"/>
     <hyperlink ref="L2" r:id="rId6" xr:uid="{FDB247FA-7FD2-4D06-8C37-1E8AB3812730}"/>
-    <hyperlink ref="L14" r:id="rId7" xr:uid="{C08E3E87-43B9-4D70-9E8C-1F9D10C0C528}"/>
+    <hyperlink ref="L15" r:id="rId7" xr:uid="{C08E3E87-43B9-4D70-9E8C-1F9D10C0C528}"/>
     <hyperlink ref="L4" r:id="rId8" xr:uid="{CEBB90C9-EE2A-4076-89E6-4175BD765AC5}"/>
     <hyperlink ref="D4" r:id="rId9" xr:uid="{2BD13B79-1C8F-467A-B33D-337078B2D965}"/>
     <hyperlink ref="D7" r:id="rId10" xr:uid="{3C7B36F5-B454-4699-B258-FE72CF6405EF}"/>
     <hyperlink ref="L6" r:id="rId11" xr:uid="{767E5B79-2C05-406C-9DF6-3188BD2AE85E}"/>
     <hyperlink ref="D10" r:id="rId12" xr:uid="{88585AB6-04B4-4393-9815-7627CA77C111}"/>
     <hyperlink ref="L7" r:id="rId13" xr:uid="{5DAE1CE9-DE22-4DC4-813D-66E80378D1AE}"/>
-    <hyperlink ref="D14" r:id="rId14" location="crypto-intraday" xr:uid="{3643EC49-1164-4528-A647-5BC0FCC8D553}"/>
+    <hyperlink ref="D15" r:id="rId14" location="crypto-intraday" xr:uid="{3643EC49-1164-4528-A647-5BC0FCC8D553}"/>
     <hyperlink ref="L9" r:id="rId15" xr:uid="{01C5E072-4DD0-40F2-BE2D-29EA52FDD444}"/>
     <hyperlink ref="L10" r:id="rId16" xr:uid="{7C91756B-6844-4587-BB63-CFBBDE213F1B}"/>
     <hyperlink ref="L11" r:id="rId17" xr:uid="{FBA1D981-7D5F-45D9-9A46-9FA9B0F995B6}"/>
     <hyperlink ref="D9" r:id="rId18" xr:uid="{D18F1F1C-575C-4EE2-BAA6-8F1B4753130D}"/>
+    <hyperlink ref="D14" r:id="rId19" xr:uid="{6D86BD27-2B1B-42D2-9BBF-6A1F0E338F2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Module Disp Logic Fix
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Work\Programming\Projects\brief-me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CC29CF-7F4F-49D4-B1FE-03C796290974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE43988-0B4A-4BB6-8D77-C53C03E0EA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,6 +192,246 @@
     <t>Updates In</t>
   </si>
   <si>
+    <t>API Website/Docs</t>
+  </si>
+  <si>
+    <t>https://gold-price-live.p.rapidapi.com/get_metal_prices?X-RapidAPI-Key=2538a292famsh640adda00593d8cp17430ejsn464f9c2d4f7a</t>
+  </si>
+  <si>
+    <t>Every 10 Minutes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Every 400 minutes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500/Day Per API </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every 12 Hours. </t>
+  </si>
+  <si>
+    <t>https://api.wikimedia.org/wiki/API_reference/Feed/On_this_day</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Every Once A Day</t>
+  </si>
+  <si>
+    <t>ghttps://api.wikimedia.org/feed/v1/wikipedia/en/onthisday/holidays/</t>
+  </si>
+  <si>
+    <t>onThisDayHoliday</t>
+  </si>
+  <si>
+    <t>onThisDayBirths</t>
+  </si>
+  <si>
+    <t>https://github.com/vedicscriptures/bhagavad-gita-api</t>
+  </si>
+  <si>
+    <t>https://bhagavadgitaapi.in/slok/3/12</t>
+  </si>
+  <si>
+    <t>Generate a random digit for the slok and the chapter.</t>
+  </si>
+  <si>
+    <t>Once a Day</t>
+  </si>
+  <si>
+    <t>Holidays</t>
+  </si>
+  <si>
+    <t>Births</t>
+  </si>
+  <si>
+    <t>chapter and slok</t>
+  </si>
+  <si>
+    <t>travelDurationTraffic, travelMode trafficCongestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">every day @ a fixed time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To and From, PIN Depart time. </t>
+  </si>
+  <si>
+    <t>https://openweathermap.org/current</t>
+  </si>
+  <si>
+    <t>AQI</t>
+  </si>
+  <si>
+    <t>https://openweathermap.org/api/air-pollution</t>
+  </si>
+  <si>
+    <t>Displays the AQI of current location.</t>
+  </si>
+  <si>
+    <t>Props to Display.</t>
+  </si>
+  <si>
+    <t>https://api.openweathermap.org/data/2.5/weather?lat={lat}&amp;lon={lon}&amp;appid={API key}</t>
+  </si>
+  <si>
+    <t>http://api.openweathermap.org/data/2.5/air_pollution?lat={lat}&amp;lon={lon}&amp;appid={API key}</t>
+  </si>
+  <si>
+    <t>60/Minute</t>
+  </si>
+  <si>
+    <t>500/Hour</t>
+  </si>
+  <si>
+    <t>5/Day</t>
+  </si>
+  <si>
+    <t>Realtime</t>
+  </si>
+  <si>
+    <t>http://dev.virtualearth.net/REST/V1/Routes?wp.0=${from}&amp;wp.1=${to}&amp;optmz=timeWithTraffic&amp;key=${bing_key}</t>
+  </si>
+  <si>
+    <t>https://www.alphavantage.co/documentation/#crypto-intraday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silver price, gold price 24k,  Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">main - Stock name, price secondary - open, high, low Down or up logo on % change         Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date &amp; Holiday                         Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date &amp; Birthday,                     Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">From &amp; To, Traffic Congestion &amp; Travel Duration                      Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place name, sky condition and Icon based on Sky condition, Tempreature, humidity etc.                           Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t>https://newscatcher.p.rapidapi.com/v1/latest_headlines?lang=en&amp;country=IN&amp;media=false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 5 headlines                           Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petrol, Diesel, CNG, LPG                           Fetched from, fetched on </t>
+  </si>
+  <si>
+    <t>ISR or SWR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SWR, 10 minutes. </t>
+  </si>
+  <si>
+    <t>ISR, 5 hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SWR, no Interval</t>
+  </si>
+  <si>
+    <t>Firebase_ID</t>
+  </si>
+  <si>
+    <t>goldPrice</t>
+  </si>
+  <si>
+    <t>stockPrice</t>
+  </si>
+  <si>
+    <t>todayHoliday</t>
+  </si>
+  <si>
+    <t>todayBirth</t>
+  </si>
+  <si>
+    <t>routeInfo</t>
+  </si>
+  <si>
+    <t>bhagwadgita</t>
+  </si>
+  <si>
+    <t>toDo</t>
+  </si>
+  <si>
+    <t>aqi</t>
+  </si>
+  <si>
+    <t>weatherNow</t>
+  </si>
+  <si>
+    <t>nationalNews</t>
+  </si>
+  <si>
+    <t>notifiers</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>telegram</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
+  <si>
+    <t>reddit</t>
+  </si>
+  <si>
+    <t>fuelPrice</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>emails</t>
+  </si>
+  <si>
+    <t>cryptoPrice</t>
+  </si>
+  <si>
+    <t>Horoscrope</t>
+  </si>
+  <si>
+    <t>Add a music widget.</t>
+  </si>
+  <si>
+    <t>Dynamic Imports</t>
+  </si>
+  <si>
+    <t>Select from DropDown menu, API…. Price IS ACTUALLY THE PREVIOUS CLOSE. Compare the low w price.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/api/rest_v1/feed/onthisday/holidays/01/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Current Time/Day</t>
+  </si>
+  <si>
+    <t>https://worldtimeapi.org/api/timezone/Asia/Kolkata</t>
+  </si>
+  <si>
+    <t>https://www.timeapi.io/api/Time/current/zone?timeZone=Asia/Kolkata</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">API Displays the 24K Rate per ounce in USD. So ((x/28.3495) * 10) * </t>
     </r>
@@ -199,7 +439,7 @@
       <rPr>
         <u/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -209,7 +449,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -217,252 +457,12 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
-  <si>
-    <t>API Website/Docs</t>
-  </si>
-  <si>
-    <t>https://gold-price-live.p.rapidapi.com/get_metal_prices?X-RapidAPI-Key=2538a292famsh640adda00593d8cp17430ejsn464f9c2d4f7a</t>
-  </si>
-  <si>
-    <t>Every 10 Minutes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Every 400 minutes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500/Day Per API </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Every 12 Hours. </t>
-  </si>
-  <si>
-    <t>https://api.wikimedia.org/wiki/API_reference/Feed/On_this_day</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Every Once A Day</t>
-  </si>
-  <si>
-    <t>ghttps://api.wikimedia.org/feed/v1/wikipedia/en/onthisday/holidays/</t>
-  </si>
-  <si>
-    <t>onThisDayHoliday</t>
-  </si>
-  <si>
-    <t>onThisDayBirths</t>
-  </si>
-  <si>
-    <t>https://github.com/vedicscriptures/bhagavad-gita-api</t>
-  </si>
-  <si>
-    <t>https://bhagavadgitaapi.in/slok/3/12</t>
-  </si>
-  <si>
-    <t>Generate a random digit for the slok and the chapter.</t>
-  </si>
-  <si>
-    <t>Once a Day</t>
-  </si>
-  <si>
-    <t>Holidays</t>
-  </si>
-  <si>
-    <t>Births</t>
-  </si>
-  <si>
-    <t>chapter and slok</t>
-  </si>
-  <si>
-    <t>travelDurationTraffic, travelMode trafficCongestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">every day @ a fixed time. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To and From, PIN Depart time. </t>
-  </si>
-  <si>
-    <t>https://openweathermap.org/current</t>
-  </si>
-  <si>
-    <t>AQI</t>
-  </si>
-  <si>
-    <t>https://openweathermap.org/api/air-pollution</t>
-  </si>
-  <si>
-    <t>Displays the AQI of current location.</t>
-  </si>
-  <si>
-    <t>Props to Display.</t>
-  </si>
-  <si>
-    <t>https://api.openweathermap.org/data/2.5/weather?lat={lat}&amp;lon={lon}&amp;appid={API key}</t>
-  </si>
-  <si>
-    <t>http://api.openweathermap.org/data/2.5/air_pollution?lat={lat}&amp;lon={lon}&amp;appid={API key}</t>
-  </si>
-  <si>
-    <t>60/Minute</t>
-  </si>
-  <si>
-    <t>500/Hour</t>
-  </si>
-  <si>
-    <t>5/Day</t>
-  </si>
-  <si>
-    <t>Realtime</t>
-  </si>
-  <si>
-    <t>http://dev.virtualearth.net/REST/V1/Routes?wp.0=${from}&amp;wp.1=${to}&amp;optmz=timeWithTraffic&amp;key=${bing_key}</t>
-  </si>
-  <si>
-    <t>https://www.alphavantage.co/documentation/#crypto-intraday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">silver price, gold price 24k,  Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t xml:space="preserve">main - Stock name, price secondary - open, high, low Down or up logo on % change         Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date &amp; Holiday                         Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date &amp; Birthday,                     Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t xml:space="preserve">From &amp; To, Traffic Congestion &amp; Travel Duration                      Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place name, sky condition and Icon based on Sky condition, Tempreature, humidity etc.                           Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t>https://newscatcher.p.rapidapi.com/v1/latest_headlines?lang=en&amp;country=IN&amp;media=false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Top 5 headlines                           Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petrol, Diesel, CNG, LPG                           Fetched from, fetched on </t>
-  </si>
-  <si>
-    <t>ISR or SWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SWR, 10 minutes. </t>
-  </si>
-  <si>
-    <t>ISR, 5 hours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SWR, no Interval</t>
-  </si>
-  <si>
-    <t>Firebase_ID</t>
-  </si>
-  <si>
-    <t>goldPrice</t>
-  </si>
-  <si>
-    <t>stockPrice</t>
-  </si>
-  <si>
-    <t>todayHoliday</t>
-  </si>
-  <si>
-    <t>todayBirth</t>
-  </si>
-  <si>
-    <t>routeInfo</t>
-  </si>
-  <si>
-    <t>bhagwadgita</t>
-  </si>
-  <si>
-    <t>toDo</t>
-  </si>
-  <si>
-    <t>aqi</t>
-  </si>
-  <si>
-    <t>weatherNow</t>
-  </si>
-  <si>
-    <t>nationalNews</t>
-  </si>
-  <si>
-    <t>notifiers</t>
-  </si>
-  <si>
-    <t>instagram</t>
-  </si>
-  <si>
-    <t>facebook</t>
-  </si>
-  <si>
-    <t>whatsapp</t>
-  </si>
-  <si>
-    <t>telegram</t>
-  </si>
-  <si>
-    <t>twitter</t>
-  </si>
-  <si>
-    <t>reddit</t>
-  </si>
-  <si>
-    <t>fuelPrice</t>
-  </si>
-  <si>
-    <t>linkedin</t>
-  </si>
-  <si>
-    <t>github</t>
-  </si>
-  <si>
-    <t>emails</t>
-  </si>
-  <si>
-    <t>cryptoPrice</t>
-  </si>
-  <si>
-    <t>Horoscrope</t>
-  </si>
-  <si>
-    <t>Add a music widget.</t>
-  </si>
-  <si>
-    <t>Dynamic Imports</t>
-  </si>
-  <si>
-    <t>Select from DropDown menu, API…. Price IS ACTUALLY THE PREVIOUS CLOSE. Compare the low w price.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/api/rest_v1/feed/onthisday/holidays/01/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time </t>
-  </si>
-  <si>
-    <t>Current Time/Day</t>
-  </si>
-  <si>
-    <t>https://worldtimeapi.org/api/timezone/Asia/Kolkata</t>
-  </si>
-  <si>
-    <t>https://www.timeapi.io/api/Time/current/zone?timeZone=Asia/Kolkata</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,14 +486,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -512,6 +504,21 @@
       <color rgb="FFCE9178"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -547,7 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -564,10 +571,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -576,8 +583,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -862,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -896,7 +912,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>36</v>
@@ -905,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>32</v>
@@ -926,56 +942,56 @@
         <v>54</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>102</v>
+      <c r="K2" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
@@ -990,7 +1006,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>13</v>
@@ -999,39 +1015,39 @@
         <v>52</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>28</v>
@@ -1040,71 +1056,71 @@
         <v>52</v>
       </c>
       <c r="J4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="N4" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>28</v>
@@ -1113,21 +1129,21 @@
         <v>52</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>8</v>
@@ -1136,10 +1152,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>26</v>
@@ -1148,24 +1164,24 @@
         <v>28</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="N7" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>9</v>
@@ -1177,7 +1193,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>13</v>
@@ -1192,36 +1208,36 @@
     </row>
     <row r="9" spans="1:14" s="8" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="J9" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>10</v>
@@ -1230,51 +1246,51 @@
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>28</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>33</v>
@@ -1289,21 +1305,21 @@
         <v>38</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>44</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
@@ -1311,23 +1327,23 @@
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E14" s="3"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>46</v>
@@ -1336,26 +1352,26 @@
         <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>53</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="17.850000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>17</v>
@@ -1364,7 +1380,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>18</v>
@@ -1373,7 +1389,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>19</v>
@@ -1387,7 +1403,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>20</v>
@@ -1396,7 +1412,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>21</v>
@@ -1405,7 +1421,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>22</v>
@@ -1414,7 +1430,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>23</v>
@@ -1423,7 +1439,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>24</v>
@@ -1432,7 +1448,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>25</v>
@@ -1441,7 +1457,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
@@ -1459,20 +1475,20 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unclean Code, But everything works -RDL doesnt
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Work\Programming\Projects\brief-me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE43988-0B4A-4BB6-8D77-C53C03E0EA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64D7336-676D-44F4-BD07-DBFACE00AA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,7 +462,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +520,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -554,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,6 +608,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -878,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,82 +1010,82 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:14" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:14" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="14" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1141,41 +1162,41 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:14" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="14" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a minor bug
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Work\Programming\Projects\brief-me\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Work\Programming\Projects\briefme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64D7336-676D-44F4-BD07-DBFACE00AA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15477FD5-48F3-4B61-89EE-5F1C1B122632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="137">
   <si>
     <t>Feature</t>
   </si>
@@ -456,6 +456,9 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>https://location.foursquare.com/developer/</t>
   </si>
 </sst>
 </file>
@@ -897,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,7 +925,7 @@
     <col min="15" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>103</v>
       </c>
@@ -966,7 +969,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>104</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="14" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>105</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>106</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>107</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>108</v>
       </c>
@@ -1161,8 +1164,11 @@
       <c r="N6" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O6" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="14" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>109</v>
       </c>
@@ -1200,7 +1206,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>110</v>
       </c>
@@ -1227,7 +1233,7 @@
       </c>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:14" s="8" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="8" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>111</v>
       </c>
@@ -1256,7 +1262,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>112</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>113</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>121</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>126</v>
       </c>
@@ -1346,7 +1352,7 @@
       <c r="E13" s="3"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>131</v>
       </c>
@@ -1362,7 +1368,7 @@
       <c r="E14" s="3"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>125</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17.850000000000001" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="17.850000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>114</v>
       </c>
@@ -1533,8 +1539,9 @@
     <hyperlink ref="L11" r:id="rId17" xr:uid="{FBA1D981-7D5F-45D9-9A46-9FA9B0F995B6}"/>
     <hyperlink ref="D9" r:id="rId18" xr:uid="{D18F1F1C-575C-4EE2-BAA6-8F1B4753130D}"/>
     <hyperlink ref="D14" r:id="rId19" xr:uid="{6D86BD27-2B1B-42D2-9BBF-6A1F0E338F2F}"/>
+    <hyperlink ref="O6" r:id="rId20" xr:uid="{4EB4693A-9878-4681-8C9B-09BE64D248CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>